<commit_message>
update : Excel Tool v0.12
</commit_message>
<xml_diff>
--- a/Assets/Data/Excels/ItemData.xlsx
+++ b/Assets/Data/Excels/ItemData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>id</t>
   </si>
@@ -33,6 +33,12 @@
     <t>itemType</t>
   </si>
   <si>
+    <t>itemList</t>
+  </si>
+  <si>
+    <t>itemDic</t>
+  </si>
+  <si>
     <t>检索id</t>
   </si>
   <si>
@@ -48,13 +54,25 @@
     <t>类型</t>
   </si>
   <si>
+    <t>列表</t>
+  </si>
+  <si>
+    <t>字典</t>
+  </si>
+  <si>
     <t>string</t>
   </si>
   <si>
     <t>int</t>
   </si>
   <si>
-    <t>enum|TheType</t>
+    <t>enum|ItemTypeEnum</t>
+  </si>
+  <si>
+    <t>List|string</t>
+  </si>
+  <si>
+    <t>Dictionary|string,string</t>
   </si>
   <si>
     <t>Alice</t>
@@ -63,19 +81,37 @@
     <t>A</t>
   </si>
   <si>
+    <t>JOJO,BABA</t>
+  </si>
+  <si>
+    <t>JOJO,BABA|BABA,KEKE</t>
+  </si>
+  <si>
     <t>Bob</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
+    <t>BABA,KEKE</t>
+  </si>
+  <si>
     <t>Carson</t>
   </si>
   <si>
+    <t>KEKE,MOMO</t>
+  </si>
+  <si>
     <t>David</t>
   </si>
   <si>
+    <t>MOMO,HEHE</t>
+  </si>
+  <si>
     <t>Ella</t>
+  </si>
+  <si>
+    <t>HEHE</t>
   </si>
 </sst>
 </file>
@@ -97,6 +133,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -106,12 +156,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -119,6 +170,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
@@ -126,18 +215,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -157,9 +254,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -180,66 +276,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -250,49 +286,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -304,48 +460,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -353,84 +467,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,15 +497,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -482,8 +509,41 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,30 +577,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -549,10 +585,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -561,133 +597,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1043,20 +1079,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="6"/>
   <cols>
     <col min="2" max="2" width="10.5555555555556" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="26.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="26.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1072,124 +1110,172 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>